<commit_message>
Add new Excel files for extracted trades and reference data
</commit_message>
<xml_diff>
--- a/extracted_trades.xlsx
+++ b/extracted_trades.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,15 +436,40 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>text</t>
+          <t>trade_date</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>metadata</t>
+          <t>value_date</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>currency</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>underlying_currency</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>counter_currency</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>spot_price</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>fixing_level</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>trade_id</t>
         </is>
@@ -453,43 +478,42 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>FOREX OPTION TERM SHEET
-Trade ID: FX20230928001
-TRADE DETAILS
-Trade Date: 28/09/2023
-Value Date: 30/09/2023
-Expiry Date: 28/12/2023
-CURRENCY DETAILS
-Currency: USD
-Underlying Currency: EUR
-Counter Currency: USD
-PRICING INFORMATION
-Spot Price: 1.0523
-Strike Price: 1.0550
-Fixing Level: 1.0535
-NOTIONAL AND PREMIUM
-Notional Amount: 1,000,000 EUR
-Premium Amount: 12,500 USD
-Premium Payment Date: 29/09/2023
-COUNTERPARTY INFORMATION
-Buyer: ABC Capital Ltd
-Seller: XYZ Bank
-Legal Entity Identifier (LEI): 7LTWFZYICNSX8D621K86
-ADDITIONAL INFORMATION
-Settlement: Cash Settlement
-Calculation Agent: XYZ Bank
-Business Day Convention: Modified Following
-Documentation: ISDA 2006</t>
+          <t>28/09/2023</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>{'type': 'pdf', 'pages': 1, 'page_metadata': [{'confidence': 0.0, 'text_blocks': 107}]}</t>
+          <t>30/09/2023</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>TEST_001</t>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>1.0523</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>1.0535</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>FX20230928001</t>
         </is>
       </c>
     </row>

</xml_diff>